<commit_message>
1. battle system 2. statge system 3. skin, passive table ready
</commit_message>
<xml_diff>
--- a/Assets/Resources/Excel/BattleShipDataExcel.xlsx
+++ b/Assets/Resources/Excel/BattleShipDataExcel.xlsx
@@ -587,7 +587,7 @@
   <dimension ref="A1:W41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -598,17 +598,18 @@
     <col min="7" max="7" width="17" customWidth="1"/>
     <col min="8" max="8" width="17.25" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
-    <col min="13" max="13" width="13.125" customWidth="1"/>
-    <col min="14" max="14" width="17.875" customWidth="1"/>
-    <col min="16" max="19" width="15.125" customWidth="1"/>
-    <col min="20" max="20" width="15.375" customWidth="1"/>
-    <col min="21" max="21" width="18" customWidth="1"/>
-    <col min="22" max="22" width="17.25" customWidth="1"/>
-    <col min="23" max="23" width="41.375" customWidth="1"/>
+    <col min="12" max="12" width="17.875" customWidth="1"/>
+    <col min="13" max="13" width="14.625" customWidth="1"/>
+    <col min="14" max="14" width="13.125" customWidth="1"/>
+    <col min="15" max="15" width="17.875" customWidth="1"/>
+    <col min="17" max="20" width="15.125" customWidth="1"/>
+    <col min="21" max="21" width="15.375" customWidth="1"/>
+    <col min="22" max="22" width="18" customWidth="1"/>
+    <col min="23" max="23" width="17.25" customWidth="1"/>
+    <col min="24" max="24" width="41.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
1. Plane Support 2. Ready to item table 3. add critical
</commit_message>
<xml_diff>
--- a/Assets/Resources/Excel/BattleShipDataExcel.xlsx
+++ b/Assets/Resources/Excel/BattleShipDataExcel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
   <si>
     <t>Rank</t>
   </si>
@@ -206,6 +206,14 @@
   </si>
   <si>
     <t>ResourceName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CriticalRate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CriticalDamage</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -584,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W41"/>
+  <dimension ref="A1:Y41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -602,14 +610,16 @@
     <col min="13" max="13" width="14.625" customWidth="1"/>
     <col min="14" max="14" width="13.125" customWidth="1"/>
     <col min="15" max="15" width="17.875" customWidth="1"/>
-    <col min="17" max="20" width="15.125" customWidth="1"/>
-    <col min="21" max="21" width="15.375" customWidth="1"/>
-    <col min="22" max="22" width="18" customWidth="1"/>
-    <col min="23" max="23" width="17.25" customWidth="1"/>
-    <col min="24" max="24" width="41.375" customWidth="1"/>
+    <col min="17" max="17" width="10.375" customWidth="1"/>
+    <col min="18" max="18" width="13.875" customWidth="1"/>
+    <col min="19" max="22" width="15.125" customWidth="1"/>
+    <col min="23" max="23" width="15.375" customWidth="1"/>
+    <col min="24" max="24" width="18" customWidth="1"/>
+    <col min="25" max="25" width="17.25" customWidth="1"/>
+    <col min="26" max="26" width="41.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -659,26 +669,32 @@
         <v>42</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="W1" s="2"/>
-    </row>
-    <row r="2" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y1" s="2"/>
+    </row>
+    <row r="2" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -728,26 +744,32 @@
         <v>30</v>
       </c>
       <c r="Q2" s="3">
+        <v>5</v>
+      </c>
+      <c r="R2" s="3">
+        <v>5</v>
+      </c>
+      <c r="S2" s="3">
         <v>2</v>
       </c>
-      <c r="R2" s="3">
-        <v>5</v>
-      </c>
-      <c r="S2" s="3">
+      <c r="T2" s="3">
+        <v>5</v>
+      </c>
+      <c r="U2" s="3">
         <v>100</v>
       </c>
-      <c r="T2" s="3">
+      <c r="V2" s="3">
         <v>100</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="W2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="X2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="W2" s="4"/>
-    </row>
-    <row r="3" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y2" s="4"/>
+    </row>
+    <row r="3" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -797,26 +819,32 @@
         <v>32</v>
       </c>
       <c r="Q3" s="3">
+        <v>5</v>
+      </c>
+      <c r="R3" s="3">
+        <v>5</v>
+      </c>
+      <c r="S3" s="3">
         <v>2</v>
       </c>
-      <c r="R3" s="3">
-        <v>5</v>
-      </c>
-      <c r="S3" s="3">
+      <c r="T3" s="3">
+        <v>5</v>
+      </c>
+      <c r="U3" s="3">
         <v>100</v>
       </c>
-      <c r="T3" s="3">
+      <c r="V3" s="3">
         <v>200</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="W3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="X3" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="W3" s="4"/>
-    </row>
-    <row r="4" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y3" s="4"/>
+    </row>
+    <row r="4" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -866,26 +894,32 @@
         <v>34</v>
       </c>
       <c r="Q4" s="3">
+        <v>5</v>
+      </c>
+      <c r="R4" s="3">
+        <v>5</v>
+      </c>
+      <c r="S4" s="3">
         <v>2</v>
       </c>
-      <c r="R4" s="3">
-        <v>5</v>
-      </c>
-      <c r="S4" s="3">
+      <c r="T4" s="3">
+        <v>5</v>
+      </c>
+      <c r="U4" s="3">
         <v>100</v>
       </c>
-      <c r="T4" s="3">
+      <c r="V4" s="3">
         <v>400</v>
       </c>
-      <c r="U4" s="4" t="s">
+      <c r="W4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="V4" s="4" t="s">
+      <c r="X4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="W4" s="4"/>
-    </row>
-    <row r="5" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y4" s="4"/>
+    </row>
+    <row r="5" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -935,26 +969,32 @@
         <v>36</v>
       </c>
       <c r="Q5" s="3">
+        <v>5</v>
+      </c>
+      <c r="R5" s="3">
+        <v>5</v>
+      </c>
+      <c r="S5" s="3">
         <v>2</v>
       </c>
-      <c r="R5" s="3">
-        <v>5</v>
-      </c>
-      <c r="S5" s="3">
+      <c r="T5" s="3">
+        <v>5</v>
+      </c>
+      <c r="U5" s="3">
         <v>100</v>
       </c>
-      <c r="T5" s="3">
+      <c r="V5" s="3">
         <v>800</v>
       </c>
-      <c r="U5" s="4" t="s">
+      <c r="W5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="V5" s="4" t="s">
+      <c r="X5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="W5" s="4"/>
-    </row>
-    <row r="6" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y5" s="4"/>
+    </row>
+    <row r="6" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1004,26 +1044,32 @@
         <v>38</v>
       </c>
       <c r="Q6" s="3">
+        <v>5</v>
+      </c>
+      <c r="R6" s="3">
+        <v>5</v>
+      </c>
+      <c r="S6" s="3">
         <v>2</v>
       </c>
-      <c r="R6" s="3">
-        <v>5</v>
-      </c>
-      <c r="S6" s="3">
+      <c r="T6" s="3">
+        <v>5</v>
+      </c>
+      <c r="U6" s="3">
         <v>100</v>
       </c>
-      <c r="T6" s="5">
+      <c r="V6" s="5">
         <v>1000</v>
       </c>
-      <c r="U6" s="4" t="s">
+      <c r="W6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="V6" s="4" t="s">
+      <c r="X6" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="W6" s="4"/>
-    </row>
-    <row r="7" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y6" s="4"/>
+    </row>
+    <row r="7" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1073,26 +1119,32 @@
         <v>40</v>
       </c>
       <c r="Q7" s="3">
+        <v>5</v>
+      </c>
+      <c r="R7" s="3">
+        <v>5</v>
+      </c>
+      <c r="S7" s="3">
         <v>2</v>
       </c>
-      <c r="R7" s="3">
-        <v>5</v>
-      </c>
-      <c r="S7" s="3">
+      <c r="T7" s="3">
+        <v>5</v>
+      </c>
+      <c r="U7" s="3">
         <v>100</v>
       </c>
-      <c r="T7" s="5">
+      <c r="V7" s="5">
         <v>1500</v>
       </c>
-      <c r="U7" s="4" t="s">
+      <c r="W7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="4" t="s">
+      <c r="X7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="W7" s="4"/>
-    </row>
-    <row r="8" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y7" s="4"/>
+    </row>
+    <row r="8" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1142,26 +1194,32 @@
         <v>42</v>
       </c>
       <c r="Q8" s="3">
+        <v>5</v>
+      </c>
+      <c r="R8" s="3">
+        <v>5</v>
+      </c>
+      <c r="S8" s="3">
         <v>2</v>
       </c>
-      <c r="R8" s="3">
-        <v>5</v>
-      </c>
-      <c r="S8" s="3">
+      <c r="T8" s="3">
+        <v>5</v>
+      </c>
+      <c r="U8" s="3">
         <v>100</v>
       </c>
-      <c r="T8" s="5">
+      <c r="V8" s="5">
         <v>2000</v>
       </c>
-      <c r="U8" s="4" t="s">
+      <c r="W8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="V8" s="4" t="s">
+      <c r="X8" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="W8" s="4"/>
-    </row>
-    <row r="9" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y8" s="4"/>
+    </row>
+    <row r="9" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1211,26 +1269,32 @@
         <v>44</v>
       </c>
       <c r="Q9" s="3">
+        <v>5</v>
+      </c>
+      <c r="R9" s="3">
+        <v>5</v>
+      </c>
+      <c r="S9" s="3">
         <v>2</v>
       </c>
-      <c r="R9" s="3">
-        <v>5</v>
-      </c>
-      <c r="S9" s="3">
+      <c r="T9" s="3">
+        <v>5</v>
+      </c>
+      <c r="U9" s="3">
         <v>100</v>
       </c>
-      <c r="T9" s="5">
+      <c r="V9" s="5">
         <v>3000</v>
       </c>
-      <c r="U9" s="4" t="s">
+      <c r="W9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="V9" s="4" t="s">
+      <c r="X9" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="W9" s="4"/>
-    </row>
-    <row r="10" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y9" s="4"/>
+    </row>
+    <row r="10" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1280,26 +1344,32 @@
         <v>46</v>
       </c>
       <c r="Q10" s="3">
+        <v>5</v>
+      </c>
+      <c r="R10" s="3">
+        <v>5</v>
+      </c>
+      <c r="S10" s="3">
         <v>2</v>
       </c>
-      <c r="R10" s="3">
-        <v>5</v>
-      </c>
-      <c r="S10" s="3">
+      <c r="T10" s="3">
+        <v>5</v>
+      </c>
+      <c r="U10" s="3">
         <v>100</v>
       </c>
-      <c r="T10" s="5">
+      <c r="V10" s="5">
         <v>4500</v>
       </c>
-      <c r="U10" s="4" t="s">
+      <c r="W10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="V10" s="4" t="s">
+      <c r="X10" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="W10" s="4"/>
-    </row>
-    <row r="11" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y10" s="4"/>
+    </row>
+    <row r="11" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -1349,26 +1419,32 @@
         <v>48</v>
       </c>
       <c r="Q11" s="3">
+        <v>5</v>
+      </c>
+      <c r="R11" s="3">
+        <v>5</v>
+      </c>
+      <c r="S11" s="3">
         <v>2</v>
       </c>
-      <c r="R11" s="3">
-        <v>5</v>
-      </c>
-      <c r="S11" s="3">
+      <c r="T11" s="3">
+        <v>5</v>
+      </c>
+      <c r="U11" s="3">
         <v>100</v>
       </c>
-      <c r="T11" s="5">
+      <c r="V11" s="5">
         <v>6500</v>
       </c>
-      <c r="U11" s="4" t="s">
+      <c r="W11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="V11" s="4" t="s">
+      <c r="X11" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="W11" s="4"/>
-    </row>
-    <row r="12" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y11" s="4"/>
+    </row>
+    <row r="12" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
@@ -1388,12 +1464,14 @@
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
-      <c r="T12" s="5"/>
-      <c r="U12" s="4"/>
-      <c r="V12" s="4"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="5"/>
       <c r="W12" s="4"/>
-    </row>
-    <row r="13" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+    </row>
+    <row r="13" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
@@ -1413,12 +1491,14 @@
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
-      <c r="T13" s="5"/>
-      <c r="U13" s="4"/>
-      <c r="V13" s="4"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="5"/>
       <c r="W13" s="4"/>
-    </row>
-    <row r="14" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+    </row>
+    <row r="14" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
@@ -1438,12 +1518,14 @@
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
-      <c r="T14" s="5"/>
-      <c r="U14" s="4"/>
-      <c r="V14" s="4"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="5"/>
       <c r="W14" s="4"/>
-    </row>
-    <row r="15" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4"/>
+    </row>
+    <row r="15" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
@@ -1463,12 +1545,14 @@
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
-      <c r="T15" s="5"/>
-      <c r="U15" s="4"/>
-      <c r="V15" s="4"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="5"/>
       <c r="W15" s="4"/>
-    </row>
-    <row r="16" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X15" s="4"/>
+      <c r="Y15" s="4"/>
+    </row>
+    <row r="16" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
@@ -1488,12 +1572,14 @@
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
       <c r="S16" s="3"/>
-      <c r="T16" s="5"/>
-      <c r="U16" s="4"/>
-      <c r="V16" s="4"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="5"/>
       <c r="W16" s="4"/>
-    </row>
-    <row r="17" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X16" s="4"/>
+      <c r="Y16" s="4"/>
+    </row>
+    <row r="17" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
@@ -1513,12 +1599,14 @@
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
       <c r="S17" s="3"/>
-      <c r="T17" s="5"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="5"/>
       <c r="W17" s="4"/>
-    </row>
-    <row r="18" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4"/>
+    </row>
+    <row r="18" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
@@ -1538,12 +1626,14 @@
       <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
       <c r="S18" s="3"/>
-      <c r="T18" s="5"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3"/>
+      <c r="V18" s="5"/>
       <c r="W18" s="4"/>
-    </row>
-    <row r="19" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X18" s="4"/>
+      <c r="Y18" s="4"/>
+    </row>
+    <row r="19" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
@@ -1563,12 +1653,14 @@
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
-      <c r="T19" s="5"/>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="5"/>
       <c r="W19" s="4"/>
-    </row>
-    <row r="20" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X19" s="4"/>
+      <c r="Y19" s="4"/>
+    </row>
+    <row r="20" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
@@ -1588,12 +1680,14 @@
       <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
-      <c r="T20" s="5"/>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="5"/>
       <c r="W20" s="4"/>
-    </row>
-    <row r="21" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X20" s="4"/>
+      <c r="Y20" s="4"/>
+    </row>
+    <row r="21" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
@@ -1613,12 +1707,14 @@
       <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
       <c r="S21" s="3"/>
-      <c r="T21" s="5"/>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="5"/>
       <c r="W21" s="4"/>
-    </row>
-    <row r="22" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X21" s="4"/>
+      <c r="Y21" s="4"/>
+    </row>
+    <row r="22" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
@@ -1638,12 +1734,14 @@
       <c r="Q22" s="3"/>
       <c r="R22" s="3"/>
       <c r="S22" s="3"/>
-      <c r="T22" s="5"/>
-      <c r="U22" s="4"/>
-      <c r="V22" s="4"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="5"/>
       <c r="W22" s="4"/>
-    </row>
-    <row r="23" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X22" s="4"/>
+      <c r="Y22" s="4"/>
+    </row>
+    <row r="23" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
@@ -1663,12 +1761,14 @@
       <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
       <c r="S23" s="3"/>
-      <c r="T23" s="5"/>
-      <c r="U23" s="4"/>
-      <c r="V23" s="4"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="5"/>
       <c r="W23" s="4"/>
-    </row>
-    <row r="24" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X23" s="4"/>
+      <c r="Y23" s="4"/>
+    </row>
+    <row r="24" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
@@ -1688,12 +1788,14 @@
       <c r="Q24" s="3"/>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
-      <c r="T24" s="5"/>
-      <c r="U24" s="4"/>
-      <c r="V24" s="4"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="5"/>
       <c r="W24" s="4"/>
-    </row>
-    <row r="25" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X24" s="4"/>
+      <c r="Y24" s="4"/>
+    </row>
+    <row r="25" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="4"/>
@@ -1713,12 +1815,14 @@
       <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
       <c r="S25" s="3"/>
-      <c r="T25" s="5"/>
-      <c r="U25" s="4"/>
-      <c r="V25" s="4"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="5"/>
       <c r="W25" s="4"/>
-    </row>
-    <row r="26" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X25" s="4"/>
+      <c r="Y25" s="4"/>
+    </row>
+    <row r="26" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="4"/>
@@ -1738,12 +1842,14 @@
       <c r="Q26" s="3"/>
       <c r="R26" s="3"/>
       <c r="S26" s="3"/>
-      <c r="T26" s="5"/>
-      <c r="U26" s="4"/>
-      <c r="V26" s="4"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="5"/>
       <c r="W26" s="4"/>
-    </row>
-    <row r="27" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X26" s="4"/>
+      <c r="Y26" s="4"/>
+    </row>
+    <row r="27" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="4"/>
@@ -1763,12 +1869,14 @@
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
       <c r="S27" s="3"/>
-      <c r="T27" s="5"/>
-      <c r="U27" s="4"/>
-      <c r="V27" s="4"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+      <c r="V27" s="5"/>
       <c r="W27" s="4"/>
-    </row>
-    <row r="28" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
+    </row>
+    <row r="28" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="4"/>
@@ -1788,12 +1896,14 @@
       <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
       <c r="S28" s="3"/>
-      <c r="T28" s="5"/>
-      <c r="U28" s="4"/>
-      <c r="V28" s="4"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="5"/>
       <c r="W28" s="4"/>
-    </row>
-    <row r="29" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
+    </row>
+    <row r="29" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="4"/>
@@ -1813,12 +1923,14 @@
       <c r="Q29" s="3"/>
       <c r="R29" s="3"/>
       <c r="S29" s="3"/>
-      <c r="T29" s="5"/>
-      <c r="U29" s="4"/>
-      <c r="V29" s="4"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="5"/>
       <c r="W29" s="4"/>
-    </row>
-    <row r="30" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+    </row>
+    <row r="30" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="4"/>
@@ -1838,12 +1950,14 @@
       <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
       <c r="S30" s="3"/>
-      <c r="T30" s="5"/>
-      <c r="U30" s="4"/>
-      <c r="V30" s="4"/>
+      <c r="T30" s="3"/>
+      <c r="U30" s="3"/>
+      <c r="V30" s="5"/>
       <c r="W30" s="4"/>
-    </row>
-    <row r="31" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X30" s="4"/>
+      <c r="Y30" s="4"/>
+    </row>
+    <row r="31" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="4"/>
@@ -1863,12 +1977,14 @@
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
       <c r="S31" s="3"/>
-      <c r="T31" s="5"/>
-      <c r="U31" s="4"/>
-      <c r="V31" s="4"/>
+      <c r="T31" s="3"/>
+      <c r="U31" s="3"/>
+      <c r="V31" s="5"/>
       <c r="W31" s="4"/>
-    </row>
-    <row r="32" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X31" s="4"/>
+      <c r="Y31" s="4"/>
+    </row>
+    <row r="32" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="4"/>
@@ -1888,12 +2004,14 @@
       <c r="Q32" s="3"/>
       <c r="R32" s="3"/>
       <c r="S32" s="3"/>
-      <c r="T32" s="5"/>
-      <c r="U32" s="4"/>
-      <c r="V32" s="4"/>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="5"/>
       <c r="W32" s="4"/>
-    </row>
-    <row r="33" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X32" s="4"/>
+      <c r="Y32" s="4"/>
+    </row>
+    <row r="33" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="4"/>
@@ -1913,12 +2031,14 @@
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
       <c r="S33" s="3"/>
-      <c r="T33" s="5"/>
-      <c r="U33" s="4"/>
-      <c r="V33" s="4"/>
+      <c r="T33" s="3"/>
+      <c r="U33" s="3"/>
+      <c r="V33" s="5"/>
       <c r="W33" s="4"/>
-    </row>
-    <row r="34" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X33" s="4"/>
+      <c r="Y33" s="4"/>
+    </row>
+    <row r="34" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="4"/>
@@ -1938,12 +2058,14 @@
       <c r="Q34" s="3"/>
       <c r="R34" s="3"/>
       <c r="S34" s="3"/>
-      <c r="T34" s="5"/>
-      <c r="U34" s="4"/>
-      <c r="V34" s="4"/>
+      <c r="T34" s="3"/>
+      <c r="U34" s="3"/>
+      <c r="V34" s="5"/>
       <c r="W34" s="4"/>
-    </row>
-    <row r="35" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X34" s="4"/>
+      <c r="Y34" s="4"/>
+    </row>
+    <row r="35" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="4"/>
@@ -1963,12 +2085,14 @@
       <c r="Q35" s="3"/>
       <c r="R35" s="3"/>
       <c r="S35" s="3"/>
-      <c r="T35" s="5"/>
-      <c r="U35" s="4"/>
-      <c r="V35" s="4"/>
+      <c r="T35" s="3"/>
+      <c r="U35" s="3"/>
+      <c r="V35" s="5"/>
       <c r="W35" s="4"/>
-    </row>
-    <row r="36" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X35" s="4"/>
+      <c r="Y35" s="4"/>
+    </row>
+    <row r="36" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="4"/>
@@ -1988,12 +2112,14 @@
       <c r="Q36" s="3"/>
       <c r="R36" s="3"/>
       <c r="S36" s="3"/>
-      <c r="T36" s="5"/>
-      <c r="U36" s="4"/>
-      <c r="V36" s="4"/>
+      <c r="T36" s="3"/>
+      <c r="U36" s="3"/>
+      <c r="V36" s="5"/>
       <c r="W36" s="4"/>
-    </row>
-    <row r="37" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X36" s="4"/>
+      <c r="Y36" s="4"/>
+    </row>
+    <row r="37" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="4"/>
@@ -2013,12 +2139,14 @@
       <c r="Q37" s="3"/>
       <c r="R37" s="3"/>
       <c r="S37" s="3"/>
-      <c r="T37" s="5"/>
-      <c r="U37" s="4"/>
-      <c r="V37" s="4"/>
+      <c r="T37" s="3"/>
+      <c r="U37" s="3"/>
+      <c r="V37" s="5"/>
       <c r="W37" s="4"/>
-    </row>
-    <row r="38" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X37" s="4"/>
+      <c r="Y37" s="4"/>
+    </row>
+    <row r="38" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="4"/>
@@ -2038,12 +2166,14 @@
       <c r="Q38" s="3"/>
       <c r="R38" s="3"/>
       <c r="S38" s="3"/>
-      <c r="T38" s="5"/>
-      <c r="U38" s="4"/>
-      <c r="V38" s="4"/>
+      <c r="T38" s="3"/>
+      <c r="U38" s="3"/>
+      <c r="V38" s="5"/>
       <c r="W38" s="4"/>
-    </row>
-    <row r="39" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X38" s="4"/>
+      <c r="Y38" s="4"/>
+    </row>
+    <row r="39" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="4"/>
@@ -2063,12 +2193,14 @@
       <c r="Q39" s="3"/>
       <c r="R39" s="3"/>
       <c r="S39" s="3"/>
-      <c r="T39" s="5"/>
-      <c r="U39" s="4"/>
-      <c r="V39" s="4"/>
+      <c r="T39" s="3"/>
+      <c r="U39" s="3"/>
+      <c r="V39" s="5"/>
       <c r="W39" s="4"/>
-    </row>
-    <row r="40" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X39" s="4"/>
+      <c r="Y39" s="4"/>
+    </row>
+    <row r="40" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="4"/>
@@ -2088,12 +2220,14 @@
       <c r="Q40" s="3"/>
       <c r="R40" s="3"/>
       <c r="S40" s="3"/>
-      <c r="T40" s="5"/>
-      <c r="U40" s="4"/>
-      <c r="V40" s="4"/>
+      <c r="T40" s="3"/>
+      <c r="U40" s="3"/>
+      <c r="V40" s="5"/>
       <c r="W40" s="4"/>
-    </row>
-    <row r="41" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X40" s="4"/>
+      <c r="Y40" s="4"/>
+    </row>
+    <row r="41" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="4"/>
@@ -2113,10 +2247,12 @@
       <c r="Q41" s="3"/>
       <c r="R41" s="3"/>
       <c r="S41" s="3"/>
-      <c r="T41" s="5"/>
-      <c r="U41" s="4"/>
-      <c r="V41" s="4"/>
+      <c r="T41" s="3"/>
+      <c r="U41" s="3"/>
+      <c r="V41" s="5"/>
       <c r="W41" s="4"/>
+      <c r="X41" s="4"/>
+      <c r="Y41" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
1. working passive system...
</commit_message>
<xml_diff>
--- a/Assets/Resources/Excel/BattleShipDataExcel.xlsx
+++ b/Assets/Resources/Excel/BattleShipDataExcel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
   <si>
     <t>Rank</t>
   </si>
@@ -158,10 +158,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Contry</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Accuracy</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -182,10 +178,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>TorpedoDefence</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>ReloadTime</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -214,6 +206,10 @@
   </si>
   <si>
     <t>CriticalDamage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Country</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -592,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y41"/>
+  <dimension ref="A1:X41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -608,18 +604,17 @@
     <col min="9" max="9" width="18" customWidth="1"/>
     <col min="12" max="12" width="17.875" customWidth="1"/>
     <col min="13" max="13" width="14.625" customWidth="1"/>
-    <col min="14" max="14" width="13.125" customWidth="1"/>
-    <col min="15" max="15" width="17.875" customWidth="1"/>
-    <col min="17" max="17" width="10.375" customWidth="1"/>
-    <col min="18" max="18" width="13.875" customWidth="1"/>
-    <col min="19" max="22" width="15.125" customWidth="1"/>
-    <col min="23" max="23" width="15.375" customWidth="1"/>
-    <col min="24" max="24" width="18" customWidth="1"/>
-    <col min="25" max="25" width="17.25" customWidth="1"/>
-    <col min="26" max="26" width="41.375" customWidth="1"/>
+    <col min="14" max="14" width="17.875" customWidth="1"/>
+    <col min="16" max="16" width="10.375" customWidth="1"/>
+    <col min="17" max="17" width="13.875" customWidth="1"/>
+    <col min="18" max="21" width="15.125" customWidth="1"/>
+    <col min="22" max="22" width="15.375" customWidth="1"/>
+    <col min="23" max="23" width="18" customWidth="1"/>
+    <col min="24" max="24" width="17.25" customWidth="1"/>
+    <col min="25" max="25" width="41.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -651,50 +646,47 @@
         <v>40</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>41</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="V1" s="1" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y1" s="2"/>
-    </row>
-    <row r="2" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="X1" s="2"/>
+    </row>
+    <row r="2" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -738,38 +730,35 @@
         <v>1</v>
       </c>
       <c r="O2" s="3">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="P2" s="3">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="Q2" s="3">
         <v>5</v>
       </c>
       <c r="R2" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="S2" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="T2" s="3">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="U2" s="3">
         <v>100</v>
       </c>
-      <c r="V2" s="3">
-        <v>100</v>
+      <c r="V2" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="X2" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y2" s="4"/>
-    </row>
-    <row r="3" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="X2" s="4"/>
+    </row>
+    <row r="3" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -813,38 +802,35 @@
         <v>2</v>
       </c>
       <c r="O3" s="3">
+        <v>32</v>
+      </c>
+      <c r="P3" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>5</v>
+      </c>
+      <c r="R3" s="3">
         <v>2</v>
       </c>
-      <c r="P3" s="3">
-        <v>32</v>
-      </c>
-      <c r="Q3" s="3">
-        <v>5</v>
-      </c>
-      <c r="R3" s="3">
-        <v>5</v>
-      </c>
       <c r="S3" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="T3" s="3">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="U3" s="3">
-        <v>100</v>
-      </c>
-      <c r="V3" s="3">
         <v>200</v>
       </c>
+      <c r="V3" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="W3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="X3" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y3" s="4"/>
-    </row>
-    <row r="4" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="X3" s="4"/>
+    </row>
+    <row r="4" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -885,41 +871,38 @@
         <v>0</v>
       </c>
       <c r="N4" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O4" s="3">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="P4" s="3">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="Q4" s="3">
         <v>5</v>
       </c>
       <c r="R4" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="S4" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="T4" s="3">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="U4" s="3">
-        <v>100</v>
-      </c>
-      <c r="V4" s="3">
         <v>400</v>
       </c>
+      <c r="V4" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="W4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="X4" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y4" s="4"/>
-    </row>
-    <row r="5" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="X4" s="4"/>
+    </row>
+    <row r="5" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -960,41 +943,38 @@
         <v>0</v>
       </c>
       <c r="N5" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O5" s="3">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="P5" s="3">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="Q5" s="3">
         <v>5</v>
       </c>
       <c r="R5" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="S5" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="T5" s="3">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="U5" s="3">
-        <v>100</v>
-      </c>
-      <c r="V5" s="3">
         <v>800</v>
       </c>
+      <c r="V5" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="W5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y5" s="4"/>
-    </row>
-    <row r="6" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="X5" s="4"/>
+    </row>
+    <row r="6" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1035,41 +1015,38 @@
         <v>0</v>
       </c>
       <c r="N6" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6" s="3">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="P6" s="3">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="Q6" s="3">
         <v>5</v>
       </c>
       <c r="R6" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="S6" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="T6" s="3">
-        <v>5</v>
-      </c>
-      <c r="U6" s="3">
         <v>100</v>
       </c>
-      <c r="V6" s="5">
+      <c r="U6" s="5">
         <v>1000</v>
       </c>
+      <c r="V6" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="W6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="X6" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y6" s="4"/>
-    </row>
-    <row r="7" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="X6" s="4"/>
+    </row>
+    <row r="7" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1110,41 +1087,38 @@
         <v>0</v>
       </c>
       <c r="N7" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O7" s="3">
+        <v>40</v>
+      </c>
+      <c r="P7" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>5</v>
+      </c>
+      <c r="R7" s="3">
         <v>2</v>
       </c>
-      <c r="P7" s="3">
-        <v>40</v>
-      </c>
-      <c r="Q7" s="3">
-        <v>5</v>
-      </c>
-      <c r="R7" s="3">
-        <v>5</v>
-      </c>
       <c r="S7" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="T7" s="3">
-        <v>5</v>
-      </c>
-      <c r="U7" s="3">
         <v>100</v>
       </c>
-      <c r="V7" s="5">
+      <c r="U7" s="5">
         <v>1500</v>
       </c>
+      <c r="V7" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="W7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="X7" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y7" s="4"/>
-    </row>
-    <row r="8" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="X7" s="4"/>
+    </row>
+    <row r="8" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1185,41 +1159,38 @@
         <v>0</v>
       </c>
       <c r="N8" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O8" s="3">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="P8" s="3">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="Q8" s="3">
         <v>5</v>
       </c>
       <c r="R8" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="S8" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="T8" s="3">
-        <v>5</v>
-      </c>
-      <c r="U8" s="3">
         <v>100</v>
       </c>
-      <c r="V8" s="5">
+      <c r="U8" s="5">
         <v>2000</v>
       </c>
+      <c r="V8" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="W8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="X8" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y8" s="4"/>
-    </row>
-    <row r="9" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="X8" s="4"/>
+    </row>
+    <row r="9" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1260,41 +1231,38 @@
         <v>0</v>
       </c>
       <c r="N9" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O9" s="3">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="P9" s="3">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="Q9" s="3">
         <v>5</v>
       </c>
       <c r="R9" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="S9" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="T9" s="3">
-        <v>5</v>
-      </c>
-      <c r="U9" s="3">
         <v>100</v>
       </c>
-      <c r="V9" s="5">
+      <c r="U9" s="5">
         <v>3000</v>
       </c>
+      <c r="V9" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="W9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="X9" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y9" s="4"/>
-    </row>
-    <row r="10" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="X9" s="4"/>
+    </row>
+    <row r="10" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1335,41 +1303,38 @@
         <v>0</v>
       </c>
       <c r="N10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10" s="3">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="P10" s="3">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="Q10" s="3">
         <v>5</v>
       </c>
       <c r="R10" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="S10" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="T10" s="3">
-        <v>5</v>
-      </c>
-      <c r="U10" s="3">
         <v>100</v>
       </c>
-      <c r="V10" s="5">
+      <c r="U10" s="5">
         <v>4500</v>
       </c>
+      <c r="V10" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="W10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="X10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y10" s="4"/>
-    </row>
-    <row r="11" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="X10" s="4"/>
+    </row>
+    <row r="11" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -1410,41 +1375,38 @@
         <v>0</v>
       </c>
       <c r="N11" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O11" s="3">
+        <v>48</v>
+      </c>
+      <c r="P11" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>5</v>
+      </c>
+      <c r="R11" s="3">
         <v>2</v>
       </c>
-      <c r="P11" s="3">
-        <v>48</v>
-      </c>
-      <c r="Q11" s="3">
-        <v>5</v>
-      </c>
-      <c r="R11" s="3">
-        <v>5</v>
-      </c>
       <c r="S11" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="T11" s="3">
-        <v>5</v>
-      </c>
-      <c r="U11" s="3">
         <v>100</v>
       </c>
-      <c r="V11" s="5">
+      <c r="U11" s="5">
         <v>6500</v>
       </c>
+      <c r="V11" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="W11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="X11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y11" s="4"/>
-    </row>
-    <row r="12" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="X11" s="4"/>
+    </row>
+    <row r="12" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
@@ -1465,13 +1427,12 @@
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
-      <c r="V12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="4"/>
       <c r="W12" s="4"/>
       <c r="X12" s="4"/>
-      <c r="Y12" s="4"/>
-    </row>
-    <row r="13" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
@@ -1492,13 +1453,12 @@
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-      <c r="V13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="4"/>
       <c r="W13" s="4"/>
       <c r="X13" s="4"/>
-      <c r="Y13" s="4"/>
-    </row>
-    <row r="14" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
@@ -1519,13 +1479,12 @@
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="4"/>
       <c r="W14" s="4"/>
       <c r="X14" s="4"/>
-      <c r="Y14" s="4"/>
-    </row>
-    <row r="15" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
@@ -1546,13 +1505,12 @@
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
-      <c r="V15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="4"/>
       <c r="W15" s="4"/>
       <c r="X15" s="4"/>
-      <c r="Y15" s="4"/>
-    </row>
-    <row r="16" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
@@ -1573,13 +1531,12 @@
       <c r="R16" s="3"/>
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
-      <c r="V16" s="5"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="4"/>
       <c r="W16" s="4"/>
       <c r="X16" s="4"/>
-      <c r="Y16" s="4"/>
-    </row>
-    <row r="17" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
@@ -1600,13 +1557,12 @@
       <c r="R17" s="3"/>
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
-      <c r="V17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="4"/>
       <c r="W17" s="4"/>
       <c r="X17" s="4"/>
-      <c r="Y17" s="4"/>
-    </row>
-    <row r="18" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
@@ -1627,13 +1583,12 @@
       <c r="R18" s="3"/>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
-      <c r="V18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="4"/>
       <c r="W18" s="4"/>
       <c r="X18" s="4"/>
-      <c r="Y18" s="4"/>
-    </row>
-    <row r="19" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
@@ -1654,13 +1609,12 @@
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
-      <c r="V19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="4"/>
       <c r="W19" s="4"/>
       <c r="X19" s="4"/>
-      <c r="Y19" s="4"/>
-    </row>
-    <row r="20" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
@@ -1681,13 +1635,12 @@
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
-      <c r="V20" s="5"/>
+      <c r="U20" s="5"/>
+      <c r="V20" s="4"/>
       <c r="W20" s="4"/>
       <c r="X20" s="4"/>
-      <c r="Y20" s="4"/>
-    </row>
-    <row r="21" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
@@ -1708,13 +1661,12 @@
       <c r="R21" s="3"/>
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
-      <c r="V21" s="5"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="4"/>
       <c r="W21" s="4"/>
       <c r="X21" s="4"/>
-      <c r="Y21" s="4"/>
-    </row>
-    <row r="22" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
@@ -1735,13 +1687,12 @@
       <c r="R22" s="3"/>
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
-      <c r="U22" s="3"/>
-      <c r="V22" s="5"/>
+      <c r="U22" s="5"/>
+      <c r="V22" s="4"/>
       <c r="W22" s="4"/>
       <c r="X22" s="4"/>
-      <c r="Y22" s="4"/>
-    </row>
-    <row r="23" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
@@ -1755,20 +1706,19 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
+      <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
-      <c r="V23" s="5"/>
+      <c r="U23" s="5"/>
+      <c r="V23" s="4"/>
       <c r="W23" s="4"/>
       <c r="X23" s="4"/>
-      <c r="Y23" s="4"/>
-    </row>
-    <row r="24" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
@@ -1782,20 +1732,19 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
+      <c r="N24" s="3"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
-      <c r="U24" s="3"/>
-      <c r="V24" s="5"/>
+      <c r="U24" s="5"/>
+      <c r="V24" s="4"/>
       <c r="W24" s="4"/>
       <c r="X24" s="4"/>
-      <c r="Y24" s="4"/>
-    </row>
-    <row r="25" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="4"/>
@@ -1809,20 +1758,19 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
+      <c r="N25" s="3"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
-      <c r="U25" s="3"/>
-      <c r="V25" s="5"/>
+      <c r="U25" s="5"/>
+      <c r="V25" s="4"/>
       <c r="W25" s="4"/>
       <c r="X25" s="4"/>
-      <c r="Y25" s="4"/>
-    </row>
-    <row r="26" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="4"/>
@@ -1836,20 +1784,19 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
+      <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
       <c r="R26" s="3"/>
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
-      <c r="U26" s="3"/>
-      <c r="V26" s="5"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="4"/>
       <c r="W26" s="4"/>
       <c r="X26" s="4"/>
-      <c r="Y26" s="4"/>
-    </row>
-    <row r="27" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="4"/>
@@ -1863,20 +1810,19 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
+      <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
-      <c r="U27" s="3"/>
-      <c r="V27" s="5"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="4"/>
       <c r="W27" s="4"/>
       <c r="X27" s="4"/>
-      <c r="Y27" s="4"/>
-    </row>
-    <row r="28" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="4"/>
@@ -1890,20 +1836,19 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
-      <c r="N28" s="5"/>
+      <c r="N28" s="3"/>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
-      <c r="U28" s="3"/>
-      <c r="V28" s="5"/>
+      <c r="U28" s="5"/>
+      <c r="V28" s="4"/>
       <c r="W28" s="4"/>
       <c r="X28" s="4"/>
-      <c r="Y28" s="4"/>
-    </row>
-    <row r="29" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="4"/>
@@ -1917,20 +1862,19 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
+      <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
       <c r="Q29" s="3"/>
       <c r="R29" s="3"/>
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
-      <c r="U29" s="3"/>
-      <c r="V29" s="5"/>
+      <c r="U29" s="5"/>
+      <c r="V29" s="4"/>
       <c r="W29" s="4"/>
       <c r="X29" s="4"/>
-      <c r="Y29" s="4"/>
-    </row>
-    <row r="30" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="4"/>
@@ -1944,20 +1888,19 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
       <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
+      <c r="N30" s="3"/>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
-      <c r="U30" s="3"/>
-      <c r="V30" s="5"/>
+      <c r="U30" s="5"/>
+      <c r="V30" s="4"/>
       <c r="W30" s="4"/>
       <c r="X30" s="4"/>
-      <c r="Y30" s="4"/>
-    </row>
-    <row r="31" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="4"/>
@@ -1971,20 +1914,19 @@
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
       <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
+      <c r="N31" s="3"/>
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
-      <c r="U31" s="3"/>
-      <c r="V31" s="5"/>
+      <c r="U31" s="5"/>
+      <c r="V31" s="4"/>
       <c r="W31" s="4"/>
       <c r="X31" s="4"/>
-      <c r="Y31" s="4"/>
-    </row>
-    <row r="32" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="4"/>
@@ -1998,20 +1940,19 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
       <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
+      <c r="N32" s="3"/>
       <c r="O32" s="3"/>
       <c r="P32" s="3"/>
       <c r="Q32" s="3"/>
       <c r="R32" s="3"/>
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
-      <c r="U32" s="3"/>
-      <c r="V32" s="5"/>
+      <c r="U32" s="5"/>
+      <c r="V32" s="4"/>
       <c r="W32" s="4"/>
       <c r="X32" s="4"/>
-      <c r="Y32" s="4"/>
-    </row>
-    <row r="33" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="4"/>
@@ -2025,20 +1966,19 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
       <c r="M33" s="5"/>
-      <c r="N33" s="5"/>
+      <c r="N33" s="3"/>
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
-      <c r="U33" s="3"/>
-      <c r="V33" s="5"/>
+      <c r="U33" s="5"/>
+      <c r="V33" s="4"/>
       <c r="W33" s="4"/>
       <c r="X33" s="4"/>
-      <c r="Y33" s="4"/>
-    </row>
-    <row r="34" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="4"/>
@@ -2052,20 +1992,19 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
       <c r="M34" s="5"/>
-      <c r="N34" s="5"/>
+      <c r="N34" s="3"/>
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
       <c r="Q34" s="3"/>
       <c r="R34" s="3"/>
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
-      <c r="U34" s="3"/>
-      <c r="V34" s="5"/>
+      <c r="U34" s="5"/>
+      <c r="V34" s="4"/>
       <c r="W34" s="4"/>
       <c r="X34" s="4"/>
-      <c r="Y34" s="4"/>
-    </row>
-    <row r="35" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="4"/>
@@ -2079,20 +2018,19 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
       <c r="M35" s="5"/>
-      <c r="N35" s="5"/>
+      <c r="N35" s="3"/>
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
       <c r="Q35" s="3"/>
       <c r="R35" s="3"/>
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
-      <c r="U35" s="3"/>
-      <c r="V35" s="5"/>
+      <c r="U35" s="5"/>
+      <c r="V35" s="4"/>
       <c r="W35" s="4"/>
       <c r="X35" s="4"/>
-      <c r="Y35" s="4"/>
-    </row>
-    <row r="36" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="4"/>
@@ -2106,20 +2044,19 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
-      <c r="N36" s="5"/>
+      <c r="N36" s="3"/>
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
       <c r="Q36" s="3"/>
       <c r="R36" s="3"/>
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
-      <c r="U36" s="3"/>
-      <c r="V36" s="5"/>
+      <c r="U36" s="5"/>
+      <c r="V36" s="4"/>
       <c r="W36" s="4"/>
       <c r="X36" s="4"/>
-      <c r="Y36" s="4"/>
-    </row>
-    <row r="37" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="4"/>
@@ -2133,20 +2070,19 @@
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
       <c r="M37" s="5"/>
-      <c r="N37" s="5"/>
+      <c r="N37" s="3"/>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
       <c r="Q37" s="3"/>
       <c r="R37" s="3"/>
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
-      <c r="U37" s="3"/>
-      <c r="V37" s="5"/>
+      <c r="U37" s="5"/>
+      <c r="V37" s="4"/>
       <c r="W37" s="4"/>
       <c r="X37" s="4"/>
-      <c r="Y37" s="4"/>
-    </row>
-    <row r="38" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="4"/>
@@ -2160,20 +2096,19 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
       <c r="M38" s="5"/>
-      <c r="N38" s="5"/>
+      <c r="N38" s="3"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
       <c r="Q38" s="3"/>
       <c r="R38" s="3"/>
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
-      <c r="U38" s="3"/>
-      <c r="V38" s="5"/>
+      <c r="U38" s="5"/>
+      <c r="V38" s="4"/>
       <c r="W38" s="4"/>
       <c r="X38" s="4"/>
-      <c r="Y38" s="4"/>
-    </row>
-    <row r="39" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="4"/>
@@ -2187,20 +2122,19 @@
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
       <c r="M39" s="5"/>
-      <c r="N39" s="5"/>
+      <c r="N39" s="3"/>
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
       <c r="Q39" s="3"/>
       <c r="R39" s="3"/>
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
-      <c r="U39" s="3"/>
-      <c r="V39" s="5"/>
+      <c r="U39" s="5"/>
+      <c r="V39" s="4"/>
       <c r="W39" s="4"/>
       <c r="X39" s="4"/>
-      <c r="Y39" s="4"/>
-    </row>
-    <row r="40" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="4"/>
@@ -2214,20 +2148,19 @@
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
       <c r="M40" s="5"/>
-      <c r="N40" s="5"/>
+      <c r="N40" s="3"/>
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
       <c r="Q40" s="3"/>
       <c r="R40" s="3"/>
       <c r="S40" s="3"/>
       <c r="T40" s="3"/>
-      <c r="U40" s="3"/>
-      <c r="V40" s="5"/>
+      <c r="U40" s="5"/>
+      <c r="V40" s="4"/>
       <c r="W40" s="4"/>
       <c r="X40" s="4"/>
-      <c r="Y40" s="4"/>
-    </row>
-    <row r="41" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="4"/>
@@ -2241,18 +2174,17 @@
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
       <c r="M41" s="5"/>
-      <c r="N41" s="5"/>
+      <c r="N41" s="3"/>
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
       <c r="Q41" s="3"/>
       <c r="R41" s="3"/>
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
-      <c r="U41" s="3"/>
-      <c r="V41" s="5"/>
+      <c r="U41" s="5"/>
+      <c r="V41" s="4"/>
       <c r="W41" s="4"/>
       <c r="X41" s="4"/>
-      <c r="Y41" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>